<commit_message>
added ct threshold to stability analysis, updated CM template
</commit_message>
<xml_diff>
--- a/ConfusionMatrixTemplate.xlsx
+++ b/ConfusionMatrixTemplate.xlsx
@@ -1,17 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Idan\GitHub\analysis_utils\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36523629-7CBF-4EF5-976F-76E7C4A3DB6E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="1212" yWindow="1212" windowWidth="17280" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet 1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>Concept</t>
   </si>
@@ -59,9 +76,6 @@
   </si>
   <si>
     <t>Classifier based Percent</t>
-  </si>
-  <si>
-    <t>a</t>
   </si>
   <si>
     <t>Accuracy</t>
@@ -139,23 +153,23 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -164,7 +178,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -174,83 +188,382 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="9" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="10" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:Z43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="25.0"/>
-    <col customWidth="1" min="2" max="2" width="14.25"/>
-    <col customWidth="1" min="3" max="3" width="10.75"/>
-    <col customWidth="1" min="4" max="4" width="14.5"/>
-    <col customWidth="1" min="5" max="5" width="20.5"/>
-    <col customWidth="1" min="6" max="6" width="11.5"/>
-    <col customWidth="1" min="7" max="7" width="18.63"/>
-    <col customWidth="1" min="8" max="8" width="9.88"/>
-    <col customWidth="1" min="9" max="11" width="8.63"/>
-    <col customWidth="1" min="12" max="12" width="10.75"/>
-    <col customWidth="1" min="13" max="13" width="8.63"/>
-    <col customWidth="1" min="14" max="14" width="9.88"/>
-    <col customWidth="1" min="15" max="26" width="8.63"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="14.19921875" customWidth="1"/>
+    <col min="3" max="3" width="10.69921875" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
+    <col min="7" max="7" width="18.59765625" customWidth="1"/>
+    <col min="8" max="8" width="9.8984375" customWidth="1"/>
+    <col min="9" max="11" width="8.59765625" customWidth="1"/>
+    <col min="12" max="12" width="10.69921875" customWidth="1"/>
+    <col min="13" max="13" width="8.59765625" customWidth="1"/>
+    <col min="14" max="14" width="9.8984375" customWidth="1"/>
+    <col min="15" max="26" width="8.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -280,7 +593,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -310,7 +623,7 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -340,7 +653,7 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
+    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -370,7 +683,7 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -400,7 +713,7 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -430,7 +743,7 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
+    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -460,7 +773,7 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -488,7 +801,7 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -520,7 +833,7 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" ht="14.25" customHeight="1">
+    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -574,50 +887,50 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" ht="14.25" customHeight="1">
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B11" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="4" t="str">
-        <f t="shared" ref="D11:D14" si="1">C11/$C$15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E11" s="4" t="str">
+      <c r="D11" s="4" t="e">
+        <f t="shared" ref="D11:D14" si="0">C11/$C$15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E11" s="4" t="e">
         <f>C11/($C$11+$C$12)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" ref="F11:F14" si="2">IF(ISERR(D11*LOG(D11/O35,2)),0,D11*LOG(D11/O35,2))</f>
+        <f t="shared" ref="F11:F14" si="1">IF(ISERR(D11*LOG(D11/O35,2)),0,D11*LOG(D11/O35,2))</f>
         <v>0</v>
       </c>
       <c r="G11" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" ref="H11:H14" si="3">G11*F11</f>
+        <f t="shared" ref="H11:H14" si="2">G11*F11</f>
         <v>0</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K11" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="L11" s="5" t="str">
+        <v>0</v>
+      </c>
+      <c r="L11" s="5">
         <f>C11</f>
-        <v/>
-      </c>
-      <c r="M11" s="4" t="str">
-        <f t="shared" ref="M11:M14" si="4">L11/$L$15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N11" s="4" t="str">
-        <f t="shared" ref="N11:N12" si="5">L11/($L$12+$L$11)</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="4" t="e">
+        <f t="shared" ref="M11:M14" si="3">L11/$L$15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N11" s="4" t="e">
+        <f t="shared" ref="N11:N12" si="4">L11/($L$12+$L$11)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O11" s="1"/>
@@ -633,49 +946,50 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B12" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="4" t="str">
+      <c r="D12" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E12" s="6" t="e">
+        <f>C12/($C$11+$C$12)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F12" s="1">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="H12" s="1">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K12" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="L12" s="5" t="str">
+        <v>1</v>
+      </c>
+      <c r="L12" s="5">
         <f>C13</f>
-        <v/>
-      </c>
-      <c r="M12" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="M12" s="4" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N12" s="4" t="e">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N12" s="4" t="str">
-        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O12" s="1"/>
@@ -691,50 +1005,50 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
+    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B13" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="4" t="str">
+      <c r="D13" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E13" s="4" t="e">
+        <f t="shared" ref="E13:E14" si="5">C13/($C$13+$C$14)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F13" s="1">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E13" s="4" t="str">
-        <f t="shared" ref="E13:E14" si="6">C13/($C$13+$C$14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="H13" s="1">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K13" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="L13" s="5" t="str">
+        <v>0</v>
+      </c>
+      <c r="L13" s="5">
         <f>C12</f>
-        <v/>
-      </c>
-      <c r="M13" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N13" s="4" t="str">
-        <f t="shared" ref="N13:N14" si="7">L13/($L$14+$L$13)</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="4" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N13" s="4" t="e">
+        <f t="shared" ref="N13:N14" si="6">L13/($L$14+$L$13)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O13" s="1"/>
@@ -750,50 +1064,50 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" ht="14.25" customHeight="1">
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B14" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="4" t="str">
+      <c r="D14" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E14" s="4" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F14" s="1">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E14" s="4" t="str">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="H14" s="1">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="L14" s="5" t="str">
+        <v>1</v>
+      </c>
+      <c r="L14" s="5">
         <f>C14</f>
-        <v/>
-      </c>
-      <c r="M14" s="4" t="str">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N14" s="4" t="str">
-        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="4" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N14" s="4" t="e">
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O14" s="1"/>
@@ -809,7 +1123,7 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
+    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="5">
@@ -848,7 +1162,7 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
+    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -876,12 +1190,12 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" ht="14.25" customHeight="1">
+    <row r="17" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="4" t="str">
+      <c r="C17" s="4" t="e">
         <f>(C11+C14)/C15</f>
         <v>#DIV/0!</v>
       </c>
@@ -909,12 +1223,12 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" ht="14.25" customHeight="1">
+    <row r="18" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1"/>
-      <c r="C18" s="4" t="str">
+      <c r="C18" s="4" t="e">
         <f>(C17/C36)-1</f>
         <v>#DIV/0!</v>
       </c>
@@ -942,12 +1256,12 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" ht="14.25" customHeight="1">
+    <row r="19" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1"/>
-      <c r="C19" s="4" t="str">
+      <c r="C19" s="4" t="e">
         <f>(C17/(C36*C36))-1</f>
         <v>#DIV/0!</v>
       </c>
@@ -975,12 +1289,12 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" ht="14.25" customHeight="1">
+    <row r="20" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1"/>
-      <c r="C20" s="4" t="str">
+      <c r="C20" s="4" t="e">
         <f>C17-(1.96*C37/SQRT(C15))</f>
         <v>#DIV/0!</v>
       </c>
@@ -1008,12 +1322,12 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" ht="14.25" customHeight="1">
+    <row r="21" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1"/>
-      <c r="C21" s="4" t="str">
+      <c r="C21" s="4" t="e">
         <f>C20*0.95</f>
         <v>#DIV/0!</v>
       </c>
@@ -1041,7 +1355,7 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" ht="14.25" customHeight="1">
+    <row r="22" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1069,7 +1383,7 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" ht="14.25" customHeight="1">
+    <row r="23" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1097,12 +1411,12 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" ht="14.25" customHeight="1">
+    <row r="24" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="1"/>
-      <c r="C24" s="4" t="str">
+      <c r="C24" s="4" t="e">
         <f>C14/(C14+C13)</f>
         <v>#DIV/0!</v>
       </c>
@@ -1130,19 +1444,19 @@
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
     </row>
-    <row r="25" ht="14.25" customHeight="1">
+    <row r="25" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="4" t="e">
+        <f>C14/(C14+C12)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="4" t="str">
-        <f>C14/(C14+C12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E25" s="7" t="str">
+      <c r="E25" s="7" t="e">
         <f>(C25/C35)-1</f>
         <v>#DIV/0!</v>
       </c>
@@ -1168,12 +1482,12 @@
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
     </row>
-    <row r="26" ht="14.25" customHeight="1">
+    <row r="26" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1"/>
-      <c r="C26" s="4" t="str">
+      <c r="C26" s="4" t="e">
         <f>C12/(C12+C11)</f>
         <v>#DIV/0!</v>
       </c>
@@ -1201,12 +1515,12 @@
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
     </row>
-    <row r="27" ht="14.25" customHeight="1">
+    <row r="27" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1"/>
-      <c r="C27" s="4" t="str">
+      <c r="C27" s="4" t="e">
         <f>C14/(C14+C13+C12)</f>
         <v>#DIV/0!</v>
       </c>
@@ -1234,12 +1548,12 @@
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
     </row>
-    <row r="28" ht="14.25" customHeight="1">
+    <row r="28" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="9"/>
-      <c r="C28" s="10" t="str">
+      <c r="C28" s="10" t="e">
         <f>C11/(C11+C12)</f>
         <v>#DIV/0!</v>
       </c>
@@ -1267,7 +1581,7 @@
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
     </row>
-    <row r="29" ht="14.25" customHeight="1">
+    <row r="29" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1295,9 +1609,9 @@
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
     </row>
-    <row r="30" ht="14.25" customHeight="1">
+    <row r="30" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1305,14 +1619,14 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
@@ -1329,7 +1643,7 @@
       <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
     </row>
-    <row r="31" ht="14.25" customHeight="1">
+    <row r="31" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1357,7 +1671,7 @@
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
     </row>
-    <row r="32" ht="14.25" customHeight="1">
+    <row r="32" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1385,7 +1699,7 @@
       <c r="Y32" s="1"/>
       <c r="Z32" s="1"/>
     </row>
-    <row r="33" ht="14.25" customHeight="1">
+    <row r="33" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
@@ -1396,7 +1710,7 @@
         <v>10</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -1410,7 +1724,7 @@
         <v>10</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
@@ -1429,37 +1743,37 @@
       <c r="Y33" s="1"/>
       <c r="Z33" s="1"/>
     </row>
-    <row r="34" ht="14.25" customHeight="1">
+    <row r="34" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B34" s="5">
         <f>C11+C12</f>
         <v>0</v>
       </c>
-      <c r="C34" s="4" t="str">
-        <f t="shared" ref="C34:C35" si="8">B34/$C$15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D34" s="1" t="str">
-        <f t="shared" ref="D34:D35" si="9">-C34*LOG(C34,2)</f>
+      <c r="C34" s="4" t="e">
+        <f t="shared" ref="C34:C35" si="7">B34/$C$15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D34" s="1" t="e">
+        <f t="shared" ref="D34:D35" si="8">-C34*LOG(C34,2)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H34" s="5">
-        <f t="shared" ref="H34:H35" si="10">C11+C13</f>
-        <v>0</v>
-      </c>
-      <c r="I34" s="4" t="str">
-        <f t="shared" ref="I34:I35" si="11">H34/$C$15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J34" s="1" t="str">
-        <f t="shared" ref="J34:J35" si="12">-I34*LOG(I34,2)</f>
+        <f t="shared" ref="H34:H35" si="9">C11+C13</f>
+        <v>0</v>
+      </c>
+      <c r="I34" s="4" t="e">
+        <f t="shared" ref="I34:I35" si="10">H34/$C$15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J34" s="1" t="e">
+        <f t="shared" ref="J34:J35" si="11">-I34*LOG(I34,2)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K34" s="1"/>
@@ -1487,56 +1801,56 @@
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
     </row>
-    <row r="35" ht="14.25" customHeight="1">
+    <row r="35" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B35" s="5">
         <f>C15-B34</f>
         <v>0</v>
       </c>
-      <c r="C35" s="4" t="str">
+      <c r="C35" s="4" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D35" s="1" t="e">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D35" s="1" t="str">
-        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="5">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="I35" s="4" t="e">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I35" s="4" t="str">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J35" s="1" t="e">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J35" s="1" t="str">
-        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K35" s="1"/>
       <c r="L35" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M35" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="N35" s="5" t="str">
+        <v>0</v>
+      </c>
+      <c r="N35" s="5" t="e">
         <f>C34*I34*$C$15</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O35" s="4" t="str">
-        <f t="shared" ref="O35:O38" si="13">N35/$C$15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P35" s="4" t="str">
-        <f t="shared" ref="P35:P38" si="14">O35*G11</f>
+      <c r="O35" s="4" t="e">
+        <f t="shared" ref="O35:O38" si="12">N35/$C$15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P35" s="4" t="e">
+        <f t="shared" ref="P35:P38" si="13">O35*G11</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q35" s="1"/>
@@ -1550,12 +1864,12 @@
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
     </row>
-    <row r="36" ht="14.25" customHeight="1">
+    <row r="36" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B36" s="5"/>
-      <c r="C36" s="4" t="str">
+      <c r="C36" s="4" t="e">
         <f>MAX(C34,C35)</f>
         <v>#DIV/0!</v>
       </c>
@@ -1563,31 +1877,31 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H36" s="5"/>
-      <c r="I36" s="4" t="str">
+      <c r="I36" s="4" t="e">
         <f>MAX(I34,I35)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M36" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="N36" s="5" t="str">
+        <v>1</v>
+      </c>
+      <c r="N36" s="5" t="e">
         <f>C34*I35*$C$15</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O36" s="4" t="str">
+      <c r="O36" s="4" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P36" s="4" t="e">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P36" s="4" t="str">
-        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q36" s="1"/>
@@ -1601,12 +1915,12 @@
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
     </row>
-    <row r="37" ht="14.25" customHeight="1">
+    <row r="37" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B37" s="5"/>
-      <c r="C37" s="1" t="str">
+      <c r="C37" s="1" t="e">
         <f>C36*(1-C36)</f>
         <v>#DIV/0!</v>
       </c>
@@ -1614,31 +1928,31 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H37" s="5"/>
-      <c r="I37" s="1" t="str">
+      <c r="I37" s="1" t="e">
         <f>I36*(1-I36)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M37" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="N37" s="5" t="str">
+        <v>0</v>
+      </c>
+      <c r="N37" s="5" t="e">
         <f>C35*I34*$C$15</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O37" s="4" t="str">
+      <c r="O37" s="4" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P37" s="4" t="e">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P37" s="4" t="str">
-        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q37" s="1"/>
@@ -1652,9 +1966,9 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" ht="14.25" customHeight="1">
+    <row r="38" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38" s="5">
         <f>SUM(B34:B35)</f>
@@ -1665,7 +1979,7 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H38" s="5">
         <f>SUM(H34:H35)</f>
@@ -1675,21 +1989,21 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M38" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="N38" s="5" t="str">
+        <v>1</v>
+      </c>
+      <c r="N38" s="5" t="e">
         <f>C35*I35*$C$15</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O38" s="4" t="str">
+      <c r="O38" s="4" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P38" s="4" t="e">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P38" s="4" t="str">
-        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q38" s="1"/>
@@ -1703,11 +2017,11 @@
       <c r="Y38" s="1"/>
       <c r="Z38" s="1"/>
     </row>
-    <row r="39" ht="14.25" customHeight="1">
+    <row r="39" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B39" s="1" t="str">
+        <v>35</v>
+      </c>
+      <c r="B39" s="1" t="e">
         <f>SUM(D34:D35)</f>
         <v>#DIV/0!</v>
       </c>
@@ -1716,9 +2030,9 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H39" s="1" t="str">
+        <v>35</v>
+      </c>
+      <c r="H39" s="1" t="e">
         <f>SUM(J34:J35)</f>
         <v>#DIV/0!</v>
       </c>
@@ -1727,7 +2041,7 @@
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
-      <c r="N39" s="5" t="str">
+      <c r="N39" s="5" t="e">
         <f>SUM(N35:N38)</f>
         <v>#DIV/0!</v>
       </c>
@@ -1744,7 +2058,7 @@
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
     </row>
-    <row r="40" ht="14.25" customHeight="1">
+    <row r="40" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1772,9 +2086,9 @@
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
     </row>
-    <row r="41" ht="14.25" customHeight="1">
+    <row r="41" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B41" s="1">
         <f>SUM(F11:F14)</f>
@@ -1790,10 +2104,10 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M41" s="1"/>
-      <c r="N41" s="4" t="str">
+      <c r="N41" s="4" t="e">
         <f>N38/(N38+N36)</f>
         <v>#DIV/0!</v>
       </c>
@@ -1810,11 +2124,11 @@
       <c r="Y41" s="1"/>
       <c r="Z41" s="1"/>
     </row>
-    <row r="42" ht="14.25" customHeight="1">
+    <row r="42" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B42" s="11" t="str">
+        <v>38</v>
+      </c>
+      <c r="B42" s="11" t="e">
         <f>B41/B39</f>
         <v>#DIV/0!</v>
       </c>
@@ -1843,11 +2157,11 @@
       <c r="Y42" s="1"/>
       <c r="Z42" s="1"/>
     </row>
-    <row r="43" ht="14.25" customHeight="1">
+    <row r="43" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B43" s="11" t="str">
+        <v>39</v>
+      </c>
+      <c r="B43" s="11" t="e">
         <f>B41/H39</f>
         <v>#DIV/0!</v>
       </c>
@@ -1877,9 +2191,7 @@
       <c r="Z43" s="1"/>
     </row>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.0" footer="0.0" header="0.0" left="0.0" right="0.0" top="0.0"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>